<commit_message>
update :  second stage of project
</commit_message>
<xml_diff>
--- a/cad-tracker/SampleData2.xlsx
+++ b/cad-tracker/SampleData2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects  (Industry)\CAD automation implementation\cad-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10320616-222F-42F3-A685-95AAEE58ADDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C48A17B-8443-47AB-BE17-71022832E3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF7BFDF4-3805-439A-8D98-AB2AEA4383B5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EF7BFDF4-3805-439A-8D98-AB2AEA4383B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -193,6 +193,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFCF893-15BB-4534-B97A-6F25E0D70F73}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -593,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B965A3-11D5-4239-8414-BD4E52939FD5}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -607,7 +608,8 @@
     <col min="6" max="7" width="15.88671875" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -701,10 +703,10 @@
       <c r="M2">
         <v>2018</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="11">
         <v>88550000</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="11">
         <v>8890000</v>
       </c>
       <c r="P2" s="10" t="s">

</xml_diff>